<commit_message>
Update the Jupyter file
</commit_message>
<xml_diff>
--- a/results/Machine Learning Results (3600 data points - MVP).xlsx
+++ b/results/Machine Learning Results (3600 data points - MVP).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazia\Desktop\Python Udemy\GitRepo\CS3IP\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1883FB1-497C-4B43-B3BE-6591C80E6385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19947736-7CC3-4991-A64F-4C19A688D3C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9A48BAD5-1390-4A6E-955D-4139CCF62677}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{9A48BAD5-1390-4A6E-955D-4139CCF62677}"/>
   </bookViews>
   <sheets>
     <sheet name="Dep or Non-Dep Without LOSOCV" sheetId="1" r:id="rId1"/>
@@ -92,7 +92,7 @@
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="171" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -171,14 +171,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,7 +516,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="B14" sqref="B14:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,30 +527,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -576,114 +576,64 @@
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2">
-        <v>0.69144058081772997</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0.60032102728731895</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0.40107238605898099</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.48087431693989002</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0.62662702116840396</v>
-      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2">
-        <v>0.647688192586931</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0.50735809390329301</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0.38820375335120599</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.43985419198055797</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0.58976824651828597</v>
-      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2">
-        <v>0.62762705387848605</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0.47514792899408198</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0.43056300268096498</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.45175808720112498</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0.58364006471240304</v>
-      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2">
-        <v>0.47382499044707599</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0.38783749684582303</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0.82412868632707703</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0.52745367192862003</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0.55201685132619804</v>
-      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2">
-        <v>0.68112342376767199</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.58703374777975104</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.35442359249329702</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0.441992644600468</v>
-      </c>
-      <c r="F9" s="8">
-        <v>0.60820022011129704</v>
-      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="6"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -709,101 +659,51 @@
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="3">
-        <v>0.67233473442873504</v>
-      </c>
-      <c r="C14" s="2">
-        <v>0.55742725880551303</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0.39034852546916798</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.45916114790286899</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0.60939213153838301</v>
-      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="3">
-        <v>0.647879251050821</v>
-      </c>
-      <c r="C15" s="3">
-        <v>0.50784593437945702</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0.38176943699731902</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.43587389041934499</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0.58848044423329804</v>
-      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="2">
-        <v>0.62858234619793596</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0.47655786350148299</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0.43056300268096498</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.45239436619718298</v>
-      </c>
-      <c r="F16" s="3">
-        <v>0.58438212467084705</v>
-      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="2">
-        <v>0.64367596484524203</v>
-      </c>
-      <c r="C17" s="2">
-        <v>0</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0</v>
-      </c>
-      <c r="F17" s="5">
-        <v>0.5</v>
-      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="2">
-        <v>0.68303400840657202</v>
-      </c>
-      <c r="C18" s="2">
-        <v>0.58848797250859097</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0.36729222520107202</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0.45229448662924998</v>
-      </c>
-      <c r="F18" s="3">
-        <v>0.61255676858153896</v>
-      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -821,7 +721,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="B14" sqref="B14:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -831,30 +731,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -880,114 +780,64 @@
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2">
-        <v>0.60813489258062603</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0.41818181818181799</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0.13853297896702699</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.20185682737924099</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0.60813489258062603</v>
-      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2">
-        <v>0.54367002752932303</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0.41818181818181799</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0.14819598480382101</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.21754541989269699</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0.54367002752932303</v>
-      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2">
-        <v>0.56962648750291001</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0.41818181818181799</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0.169810131400395</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.23960723642450399</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0.56962648750291001</v>
-      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2">
-        <v>0.50654397975994803</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0.41818181818181799</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0.33183844080882802</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0.36748630065881899</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0.50654397975994803</v>
-      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2">
-        <v>0.595119187362253</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.41818181818181799</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.119213404887348</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0.17649801127398901</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0.595119187362253</v>
-      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -1013,101 +863,51 @@
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="2">
-        <v>0.595048989455223</v>
-      </c>
-      <c r="C14" s="2">
-        <v>0.41818181818181799</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0.14251313627492901</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.20779761676101999</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0.595048989455223</v>
-      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="2">
-        <v>0.54687729314767897</v>
-      </c>
-      <c r="C15" s="2">
-        <v>0.41818181818181799</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0.149612988247835</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.218975170924364</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0.54687729314767897</v>
-      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="2">
-        <v>0.56623854203497104</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0.41818181818181799</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0.16720594301147601</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.23748447948926199</v>
-      </c>
-      <c r="F16" s="3">
-        <v>0.56623854203497104</v>
-      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="2">
-        <v>0.58181818181818101</v>
-      </c>
-      <c r="C17" s="2">
-        <v>0</v>
-      </c>
-      <c r="D17" s="9">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0</v>
-      </c>
-      <c r="F17" s="3">
-        <v>0.58181818181818101</v>
-      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="2">
-        <v>0.59929946653600996</v>
-      </c>
-      <c r="C18" s="2">
-        <v>0.41818181818181799</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0.122726529701398</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0.181955673488543</v>
-      </c>
-      <c r="F18" s="3">
-        <v>0.59929946653600996</v>
-      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Added results for 3600 data points (2.5 days) experiment and added confusion matrices and correlation matrix for MVP and final experiment
</commit_message>
<xml_diff>
--- a/results/Machine Learning Results (3600 data points - MVP).xlsx
+++ b/results/Machine Learning Results (3600 data points - MVP).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazia\Desktop\Python Udemy\GitRepo\CS3IP\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19947736-7CC3-4991-A64F-4C19A688D3C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C738C55-BFFD-45C7-9932-7A4B1A8F196A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{9A48BAD5-1390-4A6E-955D-4139CCF62677}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9A48BAD5-1390-4A6E-955D-4139CCF62677}"/>
   </bookViews>
   <sheets>
     <sheet name="Dep or Non-Dep Without LOSOCV" sheetId="1" r:id="rId1"/>
@@ -88,11 +88,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -164,15 +162,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -516,7 +511,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:F18"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,30 +522,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -576,64 +571,114 @@
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3"/>
+      <c r="B5" s="2">
+        <v>0.73493975903614395</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.73076923076922995</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.55882352941176405</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.63333333333333297</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.70798319327730996</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
+      <c r="B6" s="2">
+        <v>0.72289156626506001</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.73913043478260798</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.59649122807017496</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.68877551020408101</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
+      <c r="B7" s="2">
+        <v>0.686746987951807</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.58823529411764697</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.60606060606060597</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.67166866746698595</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
+      <c r="B8" s="2">
+        <v>0.67469879518072196</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.59459459459459396</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.64705882352941102</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.61971830985915499</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.67046818727490998</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="6"/>
+      <c r="B9" s="2">
+        <v>0.69879518072289104</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.65517241379310298</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.55882352941176405</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.60317460317460303</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.67737094837935097</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -659,51 +704,101 @@
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="3"/>
+      <c r="B14" s="4">
+        <v>0.73493975903614395</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.73076923076922995</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.55882352941176405</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.63333333333333297</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.70798319327730996</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
+      <c r="B15" s="4">
+        <v>0.74698795180722799</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.78260869565217395</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.52941176470588203</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.63157894736842102</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.71368547418967498</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="3"/>
+      <c r="B16" s="2">
+        <v>0.66265060240963802</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.58823529411764697</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.58823529411764697</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.58823529411764697</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0.65126050420168002</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="5"/>
+      <c r="B17" s="2">
+        <v>0.65060240963855398</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.58064516129032195</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.52941176470588203</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.55384615384615299</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0.63205282112845096</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="3"/>
+      <c r="B18" s="2">
+        <v>0.69879518072289104</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.65517241379310298</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.55882352941176405</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.60317460317460303</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.67737094837935097</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -721,7 +816,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:F18"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -731,30 +826,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -780,64 +875,114 @@
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3"/>
+      <c r="B5" s="2">
+        <v>0.74025449298176504</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.23816214088941301</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.28096792096792</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.74025449298176504</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="4"/>
+      <c r="B6" s="2">
+        <v>0.51526271708089799</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.135491932310114</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.192604768968405</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.51526271708089799</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
+      <c r="B7" s="2">
+        <v>0.69697211879029997</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.230578512396694</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.28082200627655102</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.69697211879029997</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
+      <c r="B8" s="2">
+        <v>0.65558880513425899</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.304779614325068</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.33299029253574702</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.65558880513425899</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
+      <c r="B9" s="2">
+        <v>0.70496024177842298</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.22222353404171499</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.26536998355180103</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.70496024177842298</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -863,51 +1008,101 @@
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="3"/>
+      <c r="B14" s="2">
+        <v>0.75344352617079802</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.24954742227469501</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.29435766253947998</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.75344352617079802</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
+      <c r="B15" s="2">
+        <v>0.51799720481538603</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.36363636363636298</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.14378197560015701</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.198437017527926</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.51799720481538603</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="3"/>
+      <c r="B16" s="2">
+        <v>0.68134617907345096</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.236192443919716</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.28433949888495302</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0.68134617907345096</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="3"/>
+      <c r="B17" s="2">
+        <v>0.60542941906578196</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.36363636363636298</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.19557260920897199</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.238606847697756</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0.60542941906578196</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="3"/>
+      <c r="B18" s="2">
+        <v>0.72095480277298396</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.237396694214876</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.280467714104077</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.72095480277298396</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>